<commit_message>
ACUALIZACION VIAS, 10 DE JUNIO COMPLETO
</commit_message>
<xml_diff>
--- a/Vias Terrestres/Libro1(Recuperado automáticamente).xlsx
+++ b/Vias Terrestres/Libro1(Recuperado automáticamente).xlsx
@@ -5,28 +5,38 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubicacion C a D\Documentos\Primer-Semestre-24\Vias Terrestres\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Documents\Primer-Semestre-24\Vias Terrestres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5525D18-E046-417F-8B0E-2F6D502B88FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC62867-708B-4186-84F9-1D52602CDE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1860" windowWidth="17280" windowHeight="8964" xr2:uid="{A5CE36EF-852F-47DB-9D58-59354AB23256}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A5CE36EF-852F-47DB-9D58-59354AB23256}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Tipo de Carretera</t>
   </si>
@@ -56,13 +66,55 @@
   </si>
   <si>
     <t>10-20 años</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>Lunes</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>Miercoles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jueves </t>
+  </si>
+  <si>
+    <t>Sábado</t>
+  </si>
+  <si>
+    <t>Domingo</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t>Livianos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buses </t>
+  </si>
+  <si>
+    <t>C-2</t>
+  </si>
+  <si>
+    <t>C-3</t>
+  </si>
+  <si>
+    <t>T.D. TOTAL</t>
+  </si>
+  <si>
+    <t>Transito Semanal TS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +130,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -87,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -185,11 +244,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -215,9 +410,27 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -230,6 +443,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>102789</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C342450D-09EE-B1AD-82D1-0B0639DA56D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3257550" y="2226864"/>
+          <a:ext cx="2028825" cy="1078312"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,18 +793,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07B7E6B-14E7-47BC-BE1D-B1B4A03E6AD6}">
   <dimension ref="C6:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
@@ -558,7 +820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
@@ -566,13 +828,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
@@ -580,7 +842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
@@ -593,4 +855,322 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6332824-28AE-4075-93C9-2B4A648E48F0}">
+  <dimension ref="C3:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="11" width="8" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1295</v>
+      </c>
+      <c r="E5" s="16">
+        <f>D5/L5</f>
+        <v>0.7174515235457064</v>
+      </c>
+      <c r="F5" s="15">
+        <v>112</v>
+      </c>
+      <c r="G5" s="16">
+        <f>F5/L5</f>
+        <v>6.2049861495844877E-2</v>
+      </c>
+      <c r="H5" s="15">
+        <v>374</v>
+      </c>
+      <c r="I5" s="16">
+        <f>H5/L5</f>
+        <v>0.20720221606648198</v>
+      </c>
+      <c r="J5" s="15">
+        <v>24</v>
+      </c>
+      <c r="K5" s="16">
+        <f>J5/L5</f>
+        <v>1.3296398891966758E-2</v>
+      </c>
+      <c r="L5" s="17">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1291</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" ref="E6:E11" si="0">D6/L6</f>
+        <v>0.71129476584022033</v>
+      </c>
+      <c r="F6" s="15">
+        <v>108</v>
+      </c>
+      <c r="G6" s="16">
+        <f t="shared" ref="G6:G11" si="1">F6/L6</f>
+        <v>5.9504132231404959E-2</v>
+      </c>
+      <c r="H6" s="15">
+        <v>384</v>
+      </c>
+      <c r="I6" s="16">
+        <f t="shared" ref="I6:I11" si="2">H6/L6</f>
+        <v>0.21157024793388429</v>
+      </c>
+      <c r="J6" s="15">
+        <v>32</v>
+      </c>
+      <c r="K6" s="16">
+        <f t="shared" ref="K6:K11" si="3">J6/L6</f>
+        <v>1.7630853994490357E-2</v>
+      </c>
+      <c r="L6" s="17">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1220</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>0.69954128440366969</v>
+      </c>
+      <c r="F7" s="15">
+        <v>107</v>
+      </c>
+      <c r="G7" s="16">
+        <f t="shared" si="1"/>
+        <v>6.1353211009174312E-2</v>
+      </c>
+      <c r="H7" s="15">
+        <v>377</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" si="2"/>
+        <v>0.2161697247706422</v>
+      </c>
+      <c r="J7" s="15">
+        <v>40</v>
+      </c>
+      <c r="K7" s="16">
+        <f t="shared" si="3"/>
+        <v>2.2935779816513763E-2</v>
+      </c>
+      <c r="L7" s="17">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1189</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>0.69982342554443788</v>
+      </c>
+      <c r="F8" s="15">
+        <v>105</v>
+      </c>
+      <c r="G8" s="16">
+        <f t="shared" si="1"/>
+        <v>6.1801059446733371E-2</v>
+      </c>
+      <c r="H8" s="15">
+        <v>377</v>
+      </c>
+      <c r="I8" s="16">
+        <f t="shared" si="2"/>
+        <v>0.22189523248969983</v>
+      </c>
+      <c r="J8" s="15">
+        <v>28</v>
+      </c>
+      <c r="K8" s="16">
+        <f t="shared" si="3"/>
+        <v>1.6480282519128898E-2</v>
+      </c>
+      <c r="L8" s="17">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1193</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>0.68959537572254337</v>
+      </c>
+      <c r="F9" s="15">
+        <v>110</v>
+      </c>
+      <c r="G9" s="16">
+        <f t="shared" si="1"/>
+        <v>6.358381502890173E-2</v>
+      </c>
+      <c r="H9" s="15">
+        <v>383</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" si="2"/>
+        <v>0.22138728323699422</v>
+      </c>
+      <c r="J9" s="15">
+        <v>44</v>
+      </c>
+      <c r="K9" s="16">
+        <f t="shared" si="3"/>
+        <v>2.5433526011560695E-2</v>
+      </c>
+      <c r="L9" s="17">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="15">
+        <v>946</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>0.64353741496598638</v>
+      </c>
+      <c r="F10" s="15">
+        <v>125</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="1"/>
+        <v>8.5034013605442174E-2</v>
+      </c>
+      <c r="H10" s="15">
+        <v>375</v>
+      </c>
+      <c r="I10" s="16">
+        <f t="shared" si="2"/>
+        <v>0.25510204081632654</v>
+      </c>
+      <c r="J10" s="15">
+        <v>24</v>
+      </c>
+      <c r="K10" s="16">
+        <f t="shared" si="3"/>
+        <v>1.6326530612244899E-2</v>
+      </c>
+      <c r="L10" s="17">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="19">
+        <v>709</v>
+      </c>
+      <c r="E11" s="20">
+        <f t="shared" si="0"/>
+        <v>0.82441860465116279</v>
+      </c>
+      <c r="F11" s="19">
+        <v>48</v>
+      </c>
+      <c r="G11" s="20">
+        <f t="shared" si="1"/>
+        <v>5.5813953488372092E-2</v>
+      </c>
+      <c r="H11" s="19">
+        <v>96</v>
+      </c>
+      <c r="I11" s="20">
+        <f t="shared" si="2"/>
+        <v>0.11162790697674418</v>
+      </c>
+      <c r="J11" s="19">
+        <v>7</v>
+      </c>
+      <c r="K11" s="20">
+        <f t="shared" si="3"/>
+        <v>8.1395348837209301E-3</v>
+      </c>
+      <c r="L11" s="21">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="J12:K13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>